<commit_message>
ORG: Lógica de controle trabalho 1 finalizada
</commit_message>
<xml_diff>
--- a/ORG/trabalho1/mips.xlsx
+++ b/ORG/trabalho1/mips.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Caio\UFSC\3SemestreCCO\ORG\trabalho1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8C707CF0-98E4-4349-8E72-CD4786113CC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D74EBC7A-2F86-474C-8872-DC4A7EEEC971}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19695" yWindow="3030" windowWidth="16380" windowHeight="11835" xr2:uid="{84E882B6-97A6-44C5-B090-2274FBB0D3E5}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
   <si>
     <t>WR_RAM</t>
   </si>
@@ -114,6 +114,12 @@
   </si>
   <si>
     <t>1 (atualizar)</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>ok</t>
   </si>
 </sst>
 </file>
@@ -241,13 +247,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="000000"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="7" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -275,6 +274,13 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="164" formatCode="000000"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="7" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
@@ -295,16 +301,16 @@
   <autoFilter ref="B2:O13" xr:uid="{FAA87F12-3895-44AA-8089-F130E0250E10}"/>
   <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{F8A5574C-8748-4FBC-9AB6-4044A4699FE8}" name="Instrução" dataCellStyle="Célula de Verificação"/>
-    <tableColumn id="2" xr3:uid="{4C9C2DB9-1223-41FF-919E-9A5AAFA7414C}" name="Opcode" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{69DFB0C7-DB81-49BD-964D-A3CD3DE51660}" name="EN_RAM" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{C30D6F55-D30B-4894-8F1F-42D8657A0E3C}" name="WR_RAM" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{F2FD33DD-5556-4341-ADF8-20C68F92B0C6}" name="RD_RAM" dataDxfId="11"/>
-    <tableColumn id="6" xr3:uid="{3CB41D71-19B7-40FB-AFE8-0424D07BFDEB}" name="EN_PC" dataDxfId="10"/>
-    <tableColumn id="7" xr3:uid="{97AB9B5F-E7BC-4DF0-9504-F096A99E43F0}" name="WR_ACC" dataDxfId="9"/>
-    <tableColumn id="8" xr3:uid="{4C8FB788-E5D2-4EC3-83FD-E38B0AAFA210}" name="bit 1" dataDxfId="8"/>
-    <tableColumn id="9" xr3:uid="{9C92CED7-EADE-43E4-953C-CD8E0C072F28}" name="bit 0" dataDxfId="7"/>
-    <tableColumn id="10" xr3:uid="{D30F2C70-701F-490B-9B6C-CD2A896FBD6D}" name="SEL_OP2" dataDxfId="6"/>
-    <tableColumn id="11" xr3:uid="{D6B30BCF-EA9E-4191-A97F-24601A3BCD38}" name="SEL_ULA" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{4C9C2DB9-1223-41FF-919E-9A5AAFA7414C}" name="Opcode" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{69DFB0C7-DB81-49BD-964D-A3CD3DE51660}" name="EN_RAM" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{C30D6F55-D30B-4894-8F1F-42D8657A0E3C}" name="WR_RAM" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{F2FD33DD-5556-4341-ADF8-20C68F92B0C6}" name="RD_RAM" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{3CB41D71-19B7-40FB-AFE8-0424D07BFDEB}" name="EN_PC" dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{97AB9B5F-E7BC-4DF0-9504-F096A99E43F0}" name="WR_ACC" dataDxfId="7"/>
+    <tableColumn id="8" xr3:uid="{4C8FB788-E5D2-4EC3-83FD-E38B0AAFA210}" name="bit 1" dataDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{9C92CED7-EADE-43E4-953C-CD8E0C072F28}" name="bit 0" dataDxfId="5"/>
+    <tableColumn id="10" xr3:uid="{D30F2C70-701F-490B-9B6C-CD2A896FBD6D}" name="SEL_OP2" dataDxfId="4"/>
+    <tableColumn id="11" xr3:uid="{D6B30BCF-EA9E-4191-A97F-24601A3BCD38}" name="SEL_ULA" dataDxfId="3"/>
     <tableColumn id="12" xr3:uid="{C4339572-A0E8-4B00-9350-AE7D2E54D4AD}" name="EN_TEC" dataDxfId="2"/>
     <tableColumn id="13" xr3:uid="{99B2FC44-0B5B-4AEA-93BA-C7E2A6F77C75}" name="EM_MON" dataDxfId="1"/>
     <tableColumn id="14" xr3:uid="{872E5CB4-6325-4D6F-8AF3-7FFC45FEEF69}" name="SEL_JMP" dataDxfId="0"/>
@@ -610,10 +616,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{984E3411-345F-417F-8678-D99F47726E89}">
-  <dimension ref="B1:O13"/>
+  <dimension ref="B1:O14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1164,6 +1170,44 @@
       </c>
       <c r="O13" s="2">
         <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" t="s">
+        <v>27</v>
+      </c>
+      <c r="F14" t="s">
+        <v>27</v>
+      </c>
+      <c r="G14" t="s">
+        <v>27</v>
+      </c>
+      <c r="H14" t="s">
+        <v>27</v>
+      </c>
+      <c r="I14" t="s">
+        <v>28</v>
+      </c>
+      <c r="J14" t="s">
+        <v>28</v>
+      </c>
+      <c r="K14" t="s">
+        <v>28</v>
+      </c>
+      <c r="L14" t="s">
+        <v>28</v>
+      </c>
+      <c r="M14" t="s">
+        <v>28</v>
+      </c>
+      <c r="N14" t="s">
+        <v>28</v>
+      </c>
+      <c r="O14" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>